<commit_message>
feat: changed entity naming, added annotations on models, and changed the default DB to a MS SQL Server database
</commit_message>
<xml_diff>
--- a/docs/DB Schema & Functionnalities.xlsx
+++ b/docs/DB Schema & Functionnalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\22_GIT\csharp-project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA528C-B6D7-4451-B5A0-8041ADA78880}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960CDA4C-D67A-4D5E-8081-2BEE381A85BB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7410" xr2:uid="{DE256CF1-B5EC-4BF8-AF4C-38D694DA7FAF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>Field</t>
   </si>
@@ -296,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -543,24 +543,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,29 +574,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -603,10 +586,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,365 +935,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466A06A2-744C-4065-B114-DDA6B6F80E64}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="28" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
+      <c r="B14" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B15" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="22" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="23" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="28" t="s">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B20" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="30" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="22" t="s">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
+      <c r="B24" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B25" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="12" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="12" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="12" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="12" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="12" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="12" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="22" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="28" t="s">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B34" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="12" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="12" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="12" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="22" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="22"/>
+      <c r="B38" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38" s="30" t="s">
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B40" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="19" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="12" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+      <c r="B42" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="19" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="14" t="s">
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="21"/>
+      <c r="B44" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B45" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
-      <c r="B45" s="20" t="s">
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="22"/>
+      <c r="B46" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B47" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="27" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+      <c r="B48" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="28" t="s">
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="21"/>
+      <c r="B49" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B50" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="20" t="s">
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="22"/>
+      <c r="B51" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B52" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="17"/>
-      <c r="B52" s="21" t="s">
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21"/>
+      <c r="B53" s="11" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1302,19 +1322,19 @@
     <col min="4" max="4" width="64.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1322,7 +1342,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1331,67 +1351,67 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1399,31 +1419,31 @@
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
feat: added non-working config file. Added a bunch of seed data
</commit_message>
<xml_diff>
--- a/docs/DB Schema & Functionnalities.xlsx
+++ b/docs/DB Schema & Functionnalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\22_GIT\csharp-project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960CDA4C-D67A-4D5E-8081-2BEE381A85BB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1AE3AA-95F8-40E6-8058-04089496D197}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7410" xr2:uid="{DE256CF1-B5EC-4BF8-AF4C-38D694DA7FAF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>Field</t>
   </si>
@@ -587,15 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,6 +603,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -620,7 +621,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,11 +935,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466A06A2-744C-4065-B114-DDA6B6F80E64}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +957,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -965,79 +965,79 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -1045,31 +1045,31 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="18" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -1077,31 +1077,31 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="28" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -1109,55 +1109,55 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B34" s="15" t="s">
@@ -1165,126 +1165,132 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="19" t="s">
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27"/>
+      <c r="B40" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B41" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="9" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="7" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="26"/>
+      <c r="B43" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="9" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="8" t="s">
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="27"/>
+      <c r="B45" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B46" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
-      <c r="B46" s="10" t="s">
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="26"/>
+      <c r="B47" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B48" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="17" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="18" t="s">
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27"/>
+      <c r="B50" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B51" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
-      <c r="B51" s="10" t="s">
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="26"/>
+      <c r="B52" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B53" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="11" t="s">
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="27"/>
+      <c r="B54" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1292,14 +1298,14 @@
   <mergeCells count="10">
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A53:A54"/>
     <mergeCell ref="A25:A33"/>
     <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1310,8 +1316,8 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1340,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1342,7 +1348,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1351,67 +1357,67 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1419,31 +1425,31 @@
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>